<commit_message>
updates mid-PSA implementation, have to finish up defining and adding in all code for the variables
</commit_message>
<xml_diff>
--- a/results/annual.data.united.states.xlsx
+++ b/results/annual.data.united.states.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ayman\Google Drive\research\trauma\CT.neck\code\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F71571CC-6A79-404D-BB72-7472F5CACC22}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4DF6CBE-9D9A-47A5-9338-2A4CEDD7EAFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1185" yWindow="-120" windowWidth="27735" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2835" yWindow="1860" windowWidth="20865" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="47">
   <si>
     <t>ct.scan</t>
   </si>
@@ -150,25 +150,40 @@
     <t>Adjusted:</t>
   </si>
   <si>
-    <t>total increase in cost, 1 year</t>
-  </si>
-  <si>
-    <t>total increase qaly, 1 year</t>
-  </si>
-  <si>
-    <t>mortality prevented, initial month/event</t>
-  </si>
-  <si>
-    <t>strokes averted, initial month/event</t>
-  </si>
-  <si>
-    <t>n/a</t>
+    <t>Universal vs. EDC</t>
+  </si>
+  <si>
+    <t>Total cost, 1 year, in millions</t>
+  </si>
+  <si>
+    <t>Total QALY, 1 year, in thousands</t>
+  </si>
+  <si>
+    <t>Strokes, initial month event, IN THOUSANDS</t>
+  </si>
+  <si>
+    <t>Mortality, initial month event, in thousands</t>
+  </si>
+  <si>
+    <t>Strokes per 1000</t>
+  </si>
+  <si>
+    <t>Mortality per 1000</t>
+  </si>
+  <si>
+    <t>Total Cost per 1000</t>
+  </si>
+  <si>
+    <t>Total QALY per 1000</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000000000"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -198,8 +213,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -480,26 +498,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P26"/>
+  <dimension ref="A1:P37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView tabSelected="1" topLeftCell="B13" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="34" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="38.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="29.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="17" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="17.7109375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
@@ -859,7 +877,7 @@
         <v>0</v>
       </c>
       <c r="B15">
-        <f t="shared" ref="B15:J15" si="0">$B$11*B2</f>
+        <f t="shared" ref="B15:I15" si="0">$B$11*B2</f>
         <v>26455000</v>
       </c>
       <c r="C15">
@@ -891,12 +909,12 @@
         <v>0</v>
       </c>
       <c r="J15">
-        <f>$B$11*N2</f>
-        <v>3554134637093.2905</v>
+        <f>$B$11/1000*N2</f>
+        <v>3554134637.0932903</v>
       </c>
       <c r="K15">
-        <f>$B$11*O2</f>
-        <v>1507763814.0363593</v>
+        <f>$B$11/1000*O2</f>
+        <v>1507763.8140363593</v>
       </c>
       <c r="L15" t="str">
         <f>P2</f>
@@ -905,7 +923,7 @@
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16">
-        <f t="shared" ref="A16:J16" si="1">$B$11*A3</f>
+        <f t="shared" ref="A16:I16" si="1">$B$11*A3</f>
         <v>2405000</v>
       </c>
       <c r="B16">
@@ -941,12 +959,12 @@
         <v>0</v>
       </c>
       <c r="J16">
-        <f>$B$11*N3</f>
-        <v>3986890986648.8218</v>
+        <f t="shared" ref="J16:J19" si="2">$B$11/1000*N3</f>
+        <v>3986890986.6488218</v>
       </c>
       <c r="K16">
-        <f>$B$11*O3</f>
-        <v>1551562763.8100808</v>
+        <f t="shared" ref="K16:K19" si="3">$B$11/1000*O3</f>
+        <v>1551562.7638100809</v>
       </c>
       <c r="L16" t="str">
         <f>P3</f>
@@ -955,48 +973,48 @@
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17">
-        <f t="shared" ref="A17:J17" si="2">$B$11*A4</f>
+        <f t="shared" ref="A17:I17" si="4">$B$11*A4</f>
         <v>569542.47999999754</v>
       </c>
       <c r="B17">
+        <f t="shared" si="4"/>
+        <v>26455000</v>
+      </c>
+      <c r="C17">
+        <f t="shared" si="4"/>
+        <v>47885.173247904648</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="4"/>
+        <v>414511.96416209463</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="H17">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="I17">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="J17">
         <f t="shared" si="2"/>
-        <v>26455000</v>
-      </c>
-      <c r="C17">
-        <f t="shared" si="2"/>
-        <v>47885.173247904648</v>
-      </c>
-      <c r="D17">
-        <f t="shared" si="2"/>
-        <v>414511.96416209463</v>
-      </c>
-      <c r="E17">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="F17">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="G17">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="H17">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="I17">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J17">
-        <f>$B$11*N4</f>
-        <v>3227130113927.7222</v>
+        <v>3227130113.927722</v>
       </c>
       <c r="K17">
-        <f>$B$11*O4</f>
-        <v>1532948210.1562476</v>
+        <f t="shared" si="3"/>
+        <v>1532948.2101562477</v>
       </c>
       <c r="L17" t="str">
         <f>P4</f>
@@ -1005,48 +1023,48 @@
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18">
-        <f t="shared" ref="A18:J18" si="3">$B$11*A5</f>
+        <f t="shared" ref="A18:I18" si="5">$B$11*A5</f>
         <v>992091.36</v>
       </c>
       <c r="B18">
+        <f t="shared" si="5"/>
+        <v>26455000</v>
+      </c>
+      <c r="C18">
+        <f t="shared" si="5"/>
+        <v>45327.617020146456</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="5"/>
+        <v>405881.93677225331</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="H18">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="I18">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J18">
+        <f t="shared" si="2"/>
+        <v>3307857533.0912757</v>
+      </c>
+      <c r="K18">
         <f t="shared" si="3"/>
-        <v>26455000</v>
-      </c>
-      <c r="C18">
-        <f t="shared" si="3"/>
-        <v>45327.617020146456</v>
-      </c>
-      <c r="D18">
-        <f t="shared" si="3"/>
-        <v>405881.93677225331</v>
-      </c>
-      <c r="E18">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="F18">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="G18">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="H18">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="I18">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="J18">
-        <f>$B$11*N5</f>
-        <v>3307857533091.2759</v>
-      </c>
-      <c r="K18">
-        <f>$B$11*O5</f>
-        <v>1540481629.5173278</v>
+        <v>1540481.6295173278</v>
       </c>
       <c r="L18" t="str">
         <f>P5</f>
@@ -1055,177 +1073,323 @@
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19">
-        <f t="shared" ref="A19:J19" si="4">$B$11*A6</f>
+        <f t="shared" ref="A19:I19" si="6">$B$11*A6</f>
         <v>444232.36</v>
       </c>
       <c r="B19">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>26455000</v>
       </c>
       <c r="C19">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>49401.863569017289</v>
       </c>
       <c r="D19">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>419629.77110258222</v>
       </c>
       <c r="E19">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="F19">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="G19">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="H19">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="I19">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="J19">
-        <f>$B$11*N6</f>
-        <v>3267948881313.0747</v>
+        <f t="shared" si="2"/>
+        <v>3267948881.3130746</v>
       </c>
       <c r="K19">
-        <f>$B$11*O6</f>
-        <v>1528480717.2793295</v>
+        <f t="shared" si="3"/>
+        <v>1528480.7172793294</v>
       </c>
       <c r="L19" t="str">
         <f>P6</f>
         <v>mc</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B21" t="str">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B24" t="str">
         <f>L14</f>
         <v>strategy</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C24" t="s">
         <v>41</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D24" t="s">
+        <v>42</v>
+      </c>
+      <c r="E24" t="s">
+        <v>39</v>
+      </c>
+      <c r="F24" t="s">
         <v>40</v>
       </c>
-      <c r="E21" t="s">
-        <v>38</v>
-      </c>
-      <c r="F21" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B22" t="str">
-        <f t="shared" ref="B22:B26" si="5">L15</f>
-        <v>none</v>
-      </c>
-      <c r="C22" t="s">
-        <v>42</v>
-      </c>
-      <c r="D22" t="s">
-        <v>42</v>
-      </c>
-      <c r="E22" t="s">
-        <v>42</v>
-      </c>
-      <c r="F22" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B23" t="str">
-        <f t="shared" si="5"/>
-        <v>universal</v>
-      </c>
-      <c r="C23">
-        <f>$C$15-C16</f>
-        <v>14869.512952082805</v>
-      </c>
-      <c r="D23">
-        <f>$D$15-D16</f>
-        <v>50174.577847916458</v>
-      </c>
-      <c r="E23">
-        <f>K16-$K$15</f>
-        <v>43798949.773721457</v>
-      </c>
-      <c r="F23">
-        <f>K16-$K$15</f>
-        <v>43798949.773721457</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B24" t="str">
-        <f t="shared" si="5"/>
-        <v>dc</v>
-      </c>
-      <c r="C24">
-        <f t="shared" ref="C24:C26" si="6">$C$15-C17</f>
-        <v>8549.9699474476656</v>
-      </c>
-      <c r="D24">
-        <f t="shared" ref="D24:D26" si="7">$D$15-D17</f>
-        <v>28850.382262551808</v>
-      </c>
-      <c r="E24">
-        <f t="shared" ref="E24:E26" si="8">K17-$K$15</f>
-        <v>25184396.119888306</v>
-      </c>
-      <c r="F24">
-        <f t="shared" ref="F24:F26" si="9">K17-$K$15</f>
-        <v>25184396.119888306</v>
+      <c r="H24" t="s">
+        <v>15</v>
+      </c>
+      <c r="I24" t="s">
+        <v>43</v>
+      </c>
+      <c r="J24" t="s">
+        <v>44</v>
+      </c>
+      <c r="K24" t="s">
+        <v>45</v>
+      </c>
+      <c r="L24" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B25" t="str">
-        <f t="shared" si="5"/>
-        <v>edc</v>
-      </c>
-      <c r="C25">
-        <f t="shared" si="6"/>
-        <v>11107.526175205858</v>
-      </c>
-      <c r="D25">
-        <f t="shared" si="7"/>
-        <v>37480.409652393137</v>
-      </c>
-      <c r="E25">
-        <f t="shared" si="8"/>
-        <v>32717815.480968475</v>
-      </c>
-      <c r="F25">
-        <f t="shared" si="9"/>
-        <v>32717815.480968475</v>
+        <f>L15</f>
+        <v>none</v>
+      </c>
+      <c r="C25" s="2">
+        <f>C15</f>
+        <v>56435.143195352313</v>
+      </c>
+      <c r="D25" s="2">
+        <f>D15/1000</f>
+        <v>443.36234642464643</v>
+      </c>
+      <c r="E25" s="2">
+        <f>J15/1000000</f>
+        <v>3554.1346370932902</v>
+      </c>
+      <c r="F25" s="2">
+        <f>K15/1000</f>
+        <v>1507.7638140363592</v>
+      </c>
+      <c r="H25" t="s">
+        <v>19</v>
+      </c>
+      <c r="I25">
+        <f>C2*1000</f>
+        <v>23.465756006383497</v>
+      </c>
+      <c r="J25">
+        <f>D2*1000</f>
+        <v>184.35024799361599</v>
+      </c>
+      <c r="K25">
+        <f>N2</f>
+        <v>1477810.65991405</v>
+      </c>
+      <c r="L25">
+        <f>O2</f>
+        <v>626.92882080513903</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B26" t="str">
-        <f t="shared" si="5"/>
+        <f>L19</f>
         <v>mc</v>
       </c>
-      <c r="C26">
-        <f t="shared" si="6"/>
-        <v>7033.2796263350247</v>
-      </c>
-      <c r="D26">
+      <c r="C26" s="2">
+        <f>C19</f>
+        <v>49401.863569017289</v>
+      </c>
+      <c r="D26" s="2">
+        <f>D19/1000</f>
+        <v>419.6297711025822</v>
+      </c>
+      <c r="E26" s="2">
+        <f>J19/1000000</f>
+        <v>3267.9488813130747</v>
+      </c>
+      <c r="F26" s="2">
+        <f>K19/1000</f>
+        <v>1528.4807172793294</v>
+      </c>
+      <c r="H26" t="s">
+        <v>23</v>
+      </c>
+      <c r="I26">
+        <f t="shared" ref="I26:I29" si="7">C3*1000</f>
+        <v>17.283006338157801</v>
+      </c>
+      <c r="J26">
+        <f t="shared" ref="J26:J29" si="8">D3*1000</f>
+        <v>163.487637661842</v>
+      </c>
+      <c r="K26">
+        <f t="shared" ref="K26:L29" si="9">N3</f>
+        <v>1657750.9299995101</v>
+      </c>
+      <c r="L26">
+        <f t="shared" si="9"/>
+        <v>645.14044233267396</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B27" t="str">
+        <f>L17</f>
+        <v>dc</v>
+      </c>
+      <c r="C27" s="2">
+        <f>C17</f>
+        <v>47885.173247904648</v>
+      </c>
+      <c r="D27" s="2">
+        <f t="shared" ref="D27:D28" si="10">D17/1000</f>
+        <v>414.51196416209461</v>
+      </c>
+      <c r="E27" s="2">
+        <f t="shared" ref="E27:E28" si="11">J17/1000000</f>
+        <v>3227.130113927722</v>
+      </c>
+      <c r="F27" s="2">
+        <f t="shared" ref="F27:F28" si="12">K17/1000</f>
+        <v>1532.9482101562478</v>
+      </c>
+      <c r="H27" t="s">
+        <v>27</v>
+      </c>
+      <c r="I27">
         <f t="shared" si="7"/>
-        <v>23732.575322064222</v>
-      </c>
-      <c r="E26">
+        <v>19.910674947153698</v>
+      </c>
+      <c r="J27">
         <f t="shared" si="8"/>
-        <v>20716903.242970228</v>
-      </c>
-      <c r="F26">
+        <v>172.35424705284601</v>
+      </c>
+      <c r="K27">
         <f t="shared" si="9"/>
-        <v>20716903.242970228</v>
-      </c>
+        <v>1341842.04321319</v>
+      </c>
+      <c r="L27">
+        <f t="shared" si="9"/>
+        <v>637.40050318347096</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B28" t="str">
+        <f>L18</f>
+        <v>edc</v>
+      </c>
+      <c r="C28" s="2">
+        <f>C18</f>
+        <v>45327.617020146456</v>
+      </c>
+      <c r="D28" s="2">
+        <f t="shared" si="10"/>
+        <v>405.88193677225331</v>
+      </c>
+      <c r="E28" s="2">
+        <f t="shared" si="11"/>
+        <v>3307.8575330912759</v>
+      </c>
+      <c r="F28" s="2">
+        <f t="shared" si="12"/>
+        <v>1540.4816295173277</v>
+      </c>
+      <c r="H28" t="s">
+        <v>31</v>
+      </c>
+      <c r="I28">
+        <f t="shared" si="7"/>
+        <v>18.847242004218899</v>
+      </c>
+      <c r="J28">
+        <f t="shared" si="8"/>
+        <v>168.76587807578099</v>
+      </c>
+      <c r="K28">
+        <f t="shared" si="9"/>
+        <v>1375408.5376678901</v>
+      </c>
+      <c r="L28">
+        <f t="shared" si="9"/>
+        <v>640.53290208620695</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B29" t="str">
+        <f>L16</f>
+        <v>universal</v>
+      </c>
+      <c r="C29" s="2">
+        <f>C16</f>
+        <v>41565.630243269508</v>
+      </c>
+      <c r="D29" s="2">
+        <f>D16/1000</f>
+        <v>393.18776857672998</v>
+      </c>
+      <c r="E29" s="2">
+        <f>J16/1000000</f>
+        <v>3986.890986648822</v>
+      </c>
+      <c r="F29" s="2">
+        <f>K16/1000</f>
+        <v>1551.5627638100809</v>
+      </c>
+      <c r="H29" t="s">
+        <v>35</v>
+      </c>
+      <c r="I29">
+        <f t="shared" si="7"/>
+        <v>20.541315413312802</v>
+      </c>
+      <c r="J29">
+        <f t="shared" si="8"/>
+        <v>174.48223330668699</v>
+      </c>
+      <c r="K29">
+        <f t="shared" si="9"/>
+        <v>1358814.5036644801</v>
+      </c>
+      <c r="L29">
+        <f t="shared" si="9"/>
+        <v>635.54291778766299</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>38</v>
+      </c>
+      <c r="D31" s="2">
+        <f>C29-C28</f>
+        <v>-3761.9867768769473</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C32" s="1">
+        <f>E29-E28</f>
+        <v>679.03345355754618</v>
+      </c>
+      <c r="D32" s="3">
+        <f>(D29-D28)*1000</f>
+        <v>-12694.168195523333</v>
+      </c>
+      <c r="F32" s="2">
+        <f>E29-E28</f>
+        <v>679.03345355754618</v>
+      </c>
+    </row>
+    <row r="33" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C33">
+        <f>F29-F28</f>
+        <v>11.081134292753177</v>
+      </c>
+    </row>
+    <row r="37" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D37" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
final version for research letter, may include a correction on beta variables (+1 to a/b) and may need to revise the assumption sfor utiliyt of acute stroke and utility of acute trauma
</commit_message>
<xml_diff>
--- a/results/annual.data.united.states.xlsx
+++ b/results/annual.data.united.states.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ayman\Google Drive\research\trauma\CT.neck\code\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4DF6CBE-9D9A-47A5-9338-2A4CEDD7EAFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9380184E-4F16-4536-9AF1-2D0BAE6C4A15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2835" yWindow="1860" windowWidth="20865" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4065" yWindow="3120" windowWidth="20895" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="47">
   <si>
     <t>ct.scan</t>
   </si>
@@ -84,63 +84,18 @@
     <t>strategy</t>
   </si>
   <si>
-    <t>[0.18435024799361646, 0.18463111488947206, 0.1849118836146468, 0.18519255420429395, 0.18547312669355362, 0.18575360111755296, 0.186033977511406, 0.18631425591021375, 0.18659443634906417, 0.1868745188630322, 0.1871545034871797]</t>
-  </si>
-  <si>
-    <t>[793.8645120000001, 862.4408302758651, 930.9767064645504, 999.472164416307, 1067.927227967321, 1136.3419209397207, 1204.716267141586, 1273.0502903669565, 1341.344014395839, 1409.5974629942164, 1477.8106599140563]</t>
-  </si>
-  <si>
-    <t>[0.05623437056334967, 0.11339164269960397, 0.17052937972880283, 0.22764758839422522, 0.2847462754367837, 0.34182544759502526, 0.3988851116051321, 0.45592527420092266, 0.5129459421138522, 0.5699471220730139, 0.6269288208051396]</t>
-  </si>
-  <si>
     <t>none</t>
   </si>
   <si>
-    <t>[0.16348763766184213, 0.16377397476383582, 0.16406021277250893, 0.16434635172278242, 0.16463239164956453, 0.1649183325877509, 0.1652041745722245, 0.16548991763785556, 0.16577556181950182, 0.16606110715200825, 0.16634655367020723]</t>
-  </si>
-  <si>
-    <t>[1154.010688, 1204.518540510138, 1254.996606600914, 1305.4449038385226, 1355.8634497787993, 1406.2522619672263, 1456.6113579389382, 1506.9407552187286, 1557.2404713210562, 1607.5105237500507, 1657.7509299995188]</t>
-  </si>
-  <si>
-    <t>[0.05811811359527356, 0.11691033362874437, 0.17568253822418892, 0.23443473424505681, 0.2931669285524153, 0.35187912800495014, 0.41057133945896646, 0.4692435697683896, 0.5278958257847659, 0.5865281143572637, 0.645140442332674]</t>
-  </si>
-  <si>
     <t>universal</t>
   </si>
   <si>
-    <t>[0.17235424705284624, 0.17263825931723126, 0.17292217288041756, 0.17320598777742485, 0.17348970404325992, 0.1737733217129168, 0.17405684082137662, 0.17434026140360778, 0.17462358349456583, 0.17490680712919343, 0.17518993234242056]</t>
-  </si>
-  <si>
-    <t>[761.5142912000001, 819.7012416605721, 877.8538770429595, 935.9722175840811, 994.0562835089212, 1052.1060950305366, 1110.1216723500638, 1168.1030356567258, 1226.050205127839, 1283.9632009288212, 1341.8420432131973]</t>
-  </si>
-  <si>
-    <t>[0.057317522806705906, 0.1154148899838597, 0.1734924458636498, 0.23155019725845336, 0.28958815097827184, 0.34760631383073204, 0.40560469262108684, 0.4635832941522161, 0.5215421252246275, 0.5794811926364575, 0.6374005031834717]</t>
-  </si>
-  <si>
     <t>dc</t>
   </si>
   <si>
-    <t>[0.16876587807578103, 0.16905083121562178, 0.16933568549556982, 0.16962044095060486, 0.16990509761569378, 0.17018965552579082, 0.1704741147158374, 0.17075847522076218, 0.17104273707548107, 0.17132690031489728, 0.17161096497390121]</t>
-  </si>
-  <si>
-    <t>[826.076201472, 881.155375820867, 936.2020678664139, 991.2162967647021, 1046.1980816604953, 1101.1474416872672, 1156.064395967208, 1210.94896361123, 1265.801163718976, 1320.6210153788245, 1375.4085376678966]</t>
-  </si>
-  <si>
-    <t>[0.05764152660819681, 0.11602010482367184, 0.17437878912485621, 0.2327175863447964, 0.2910365033141605, 0.34933554686123913, 0.40761472381194636, 0.46587404098982044, 0.5241135052160247, 0.5823331233093485, 0.6405329020862077]</t>
-  </si>
-  <si>
     <t>edc</t>
   </si>
   <si>
-    <t>[0.17448223330668722, 0.17476568761004616, 0.17504904330631565, 0.17533230043053905, 0.17561545901774683, 0.17589851910295662, 0.17618148072117318, 0.17646434390738838, 0.17674710869658122, 0.17702977512371793, 0.17731234322375178]</t>
-  </si>
-  <si>
-    <t>[760.1057492480002, 820.1356832166763, 880.1302152290505, 940.0893661630151, 1000.0131568841504, 1059.901608245731, 1119.754741088734, 1179.572576241845, 1239.3551345214669, 1299.1024367317261, 1358.81450366448]</t>
-  </si>
-  <si>
-    <t>[0.05712538101744967, 0.11505598350908738, 0.17296682369712046, 0.23085790838166856, 0.2887292443604774, 0.3465808384289197, 0.4044126973799957, 0.46222482800433445, 0.5200172370901943, 0.577789931423464, 0.6355429177876633]</t>
-  </si>
-  <si>
     <t>mc</t>
   </si>
   <si>
@@ -175,6 +130,51 @@
   </si>
   <si>
     <t>Total QALY per 1000</t>
+  </si>
+  <si>
+    <t>[0.1838491027944195, 0.18412909000887287, 0.18440897996757075, 0.1846887727049933, 0.18496846825560798, 0.1852480666538697, 0.18552756793422076, 0.18580697213109082, 0.18608627927889695, 0.18636548941204364, 0.18664460256492274]</t>
+  </si>
+  <si>
+    <t>[687.1536, 743.6011681393054, 800.015446980947, 856.3964561569014, 912.7442152875676, 969.0587439817735, 1025.3400618367832, 1081.5881884383032, 1137.8031433604897, 1193.9849461659553, 1250.133616405776]</t>
+  </si>
+  <si>
+    <t>[0.033603881441782925, 0.08550967359198308, 0.1373977691153383, 0.18926817409512503, 0.24112089461249953, 0.2929559367464986, 0.3447733065740404, 0.39657301016992497, 0.4483550536068354, 0.5001194429553383, 0.5518661842838845]</t>
+  </si>
+  <si>
+    <t>[0.16298649246264515, 0.16327194988323662, 0.16355730912543287, 0.16384257022348175, 0.16412773321161886, 0.16441279812406762, 0.1646977649950392, 0.16498263385873257, 0.16526740474933452, 0.16555207770101957, 0.16583665274795012]</t>
+  </si>
+  <si>
+    <t>[1047.2997759999998, 1085.6788783735783, 1124.0353471173105, 1162.3691955791169, 1200.6804370990458, 1238.9690850092788, 1277.2351526341347, 1315.4786532900746, 1353.699600285706, 1391.8980069217887, 1430.0738864912373]</t>
+  </si>
+  <si>
+    <t>[0.03460196415702822, 0.0879888267552951, 0.14135755760336702, 0.19470816289338086, 0.24804064881533888, 0.3013550215571095, 0.3546512873044281, 0.4079294522408975, 0.4611895225479892, 0.5144315044050436, 0.5676554039892711]</t>
+  </si>
+  <si>
+    <t>[0.17185310185364927, 0.17213623443663206, 0.1724192692333415, 0.1727022062781242, 0.17298504560531425, 0.17326778724923353, 0.1735504312441914, 0.17383297762448488, 0.1741154264243986, 0.17439777767820486, 0.17468003142016356]</t>
+  </si>
+  <si>
+    <t>[654.8033792, 700.8615795240124, 746.8926175593562, 792.8965093246754, 838.8732708291677, 884.8229180725892, 930.7454670452605, 976.6409337280719, 1022.5093340924893, 1068.3506841005596, 1114.1649997049165]</t>
+  </si>
+  <si>
+    <t>[0.03417777900304897, 0.08693518666088748, 0.1396746474959548, 0.1923961676541221, 0.24509975327913214, 0.2977854105125999, 0.3504531454940133, 0.4031029643607342, 0.45573487324799883, 0.5083488782889188, 0.5609449856144817]</t>
+  </si>
+  <si>
+    <t>[0.16826473287658403, 0.16854880633502256, 0.16883278184849373, 0.16911665945130414, 0.16940043917774808, 0.1696841210621075, 0.1699677051386521, 0.17025119144163917, 0.17053458000531377, 0.17081787086390862, 0.17110106405164413]</t>
+  </si>
+  <si>
+    <t>[719.365289472, 762.3157136843074, 805.2408083828108, 848.1405885052966, 891.0150689807421, 933.8642647293202, 976.688190662405, 1019.4868616825765, 1062.2602926836264, 1105.0084985505628, 1147.7314941596155]</t>
+  </si>
+  <si>
+    <t>[0.034349449230071154, 0.08736160100497714, 0.14035573111589572, 0.1933318457274221, 0.2462899510020205, 0.29923005310002493, 0.35215215817963996, 0.4050562723969414, 0.4579424019058772, 0.510810552858268, 0.5636607314038081]</t>
+  </si>
+  <si>
+    <t>[0.17398108810749024, 0.17426366272944693, 0.17454613965923954, 0.17482851893123832, 0.1751108005798011, 0.1753929846392733, 0.17567507114398787, 0.17595706012826534, 0.1762389516264139, 0.1765207456727292, 0.17680244230149464]</t>
+  </si>
+  <si>
+    <t>[653.394837248, 701.2960210801166, 749.1689557454471, 797.0136579036094, 844.8301442043969, 892.6184312877837, 940.3785357839306, 988.1104743131912, 1035.8142634861172, 1083.4899199034646, 1131.1374601561993]</t>
+  </si>
+  <si>
+    <t>[0.03407597456609395, 0.08668231303822965, 0.13927074907017586, 0.19184128879670004, 0.24439393835044254, 0.29692870386191755, 0.3494455914595137, 0.40194460726949494, 0.4544257574160011, 0.5068890480210488, 0.5593344852045322]</t>
   </si>
 </sst>
 </file>
@@ -498,10 +498,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P37"/>
+  <dimension ref="A1:AE37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B13" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView tabSelected="1" topLeftCell="G13" workbookViewId="0">
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -520,7 +520,7 @@
     <col min="12" max="12" width="18.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -570,7 +570,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -578,10 +578,10 @@
         <v>11</v>
       </c>
       <c r="C2">
-        <v>2.3465756006383499E-2</v>
+        <v>1.9315485205580501E-2</v>
       </c>
       <c r="D2">
-        <v>0.18435024799361599</v>
+        <v>0.18384910279441899</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -602,25 +602,25 @@
         <v>612</v>
       </c>
       <c r="K2" t="s">
+        <v>32</v>
+      </c>
+      <c r="L2" t="s">
+        <v>33</v>
+      </c>
+      <c r="M2" t="s">
+        <v>34</v>
+      </c>
+      <c r="N2">
+        <v>1250133.6164057699</v>
+      </c>
+      <c r="O2">
+        <v>551.86618428388397</v>
+      </c>
+      <c r="P2" t="s">
         <v>16</v>
       </c>
-      <c r="L2" t="s">
-        <v>17</v>
-      </c>
-      <c r="M2" t="s">
-        <v>18</v>
-      </c>
-      <c r="N2">
-        <v>1477810.65991405</v>
-      </c>
-      <c r="O2">
-        <v>626.92882080513903</v>
-      </c>
-      <c r="P2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -628,10 +628,10 @@
         <v>11</v>
       </c>
       <c r="C3">
-        <v>1.72830063381578E-2</v>
+        <v>1.3132735537354801E-2</v>
       </c>
       <c r="D3">
-        <v>0.16348763766184199</v>
+        <v>0.16298649246264499</v>
       </c>
       <c r="E3">
         <v>0</v>
@@ -652,25 +652,25 @@
         <v>612</v>
       </c>
       <c r="K3" t="s">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="L3" t="s">
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="M3" t="s">
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="N3">
-        <v>1657750.9299995101</v>
+        <v>1430073.88649123</v>
       </c>
       <c r="O3">
-        <v>645.14044233267396</v>
+        <v>567.65540398927101</v>
       </c>
       <c r="P3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>0.236815999999999</v>
       </c>
@@ -678,10 +678,10 @@
         <v>11</v>
       </c>
       <c r="C4">
-        <v>1.9910674947153699E-2</v>
+        <v>1.5760404146350701E-2</v>
       </c>
       <c r="D4">
-        <v>0.17235424705284599</v>
+        <v>0.17185310185364899</v>
       </c>
       <c r="E4">
         <v>0</v>
@@ -702,25 +702,25 @@
         <v>612</v>
       </c>
       <c r="K4" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="L4" t="s">
-        <v>25</v>
+        <v>39</v>
       </c>
       <c r="M4" t="s">
-        <v>26</v>
+        <v>40</v>
       </c>
       <c r="N4">
-        <v>1341842.04321319</v>
+        <v>1114164.99970491</v>
       </c>
       <c r="O4">
-        <v>637.40050318347096</v>
+        <v>560.94498561448097</v>
       </c>
       <c r="P4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>0.41251199999999999</v>
       </c>
@@ -728,10 +728,10 @@
         <v>11</v>
       </c>
       <c r="C5">
-        <v>1.88472420042189E-2</v>
+        <v>1.46969712034159E-2</v>
       </c>
       <c r="D5">
-        <v>0.168765878075781</v>
+        <v>0.168264732876584</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -752,25 +752,25 @@
         <v>612</v>
       </c>
       <c r="K5" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="L5" t="s">
-        <v>29</v>
+        <v>42</v>
       </c>
       <c r="M5" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="N5">
-        <v>1375408.5376678901</v>
+        <v>1147731.49415961</v>
       </c>
       <c r="O5">
-        <v>640.53290208620695</v>
+        <v>563.66073140380797</v>
       </c>
       <c r="P5" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>0.18471199999999999</v>
       </c>
@@ -778,10 +778,10 @@
         <v>11</v>
       </c>
       <c r="C6">
-        <v>2.0541315413312802E-2</v>
+        <v>1.63910446125097E-2</v>
       </c>
       <c r="D6">
-        <v>0.174482233306687</v>
+        <v>0.17398108810749</v>
       </c>
       <c r="E6">
         <v>0</v>
@@ -802,38 +802,284 @@
         <v>612</v>
       </c>
       <c r="K6" t="s">
+        <v>44</v>
+      </c>
+      <c r="L6" t="s">
+        <v>45</v>
+      </c>
+      <c r="M6" t="s">
+        <v>46</v>
+      </c>
+      <c r="N6">
+        <v>1131137.46015619</v>
+      </c>
+      <c r="O6">
+        <v>559.33448520453203</v>
+      </c>
+      <c r="P6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="P9" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>1</v>
+      </c>
+      <c r="R9" t="s">
+        <v>2</v>
+      </c>
+      <c r="S9" t="s">
+        <v>3</v>
+      </c>
+      <c r="T9" t="s">
+        <v>4</v>
+      </c>
+      <c r="U9" t="s">
+        <v>5</v>
+      </c>
+      <c r="V9" t="s">
+        <v>6</v>
+      </c>
+      <c r="W9" t="s">
+        <v>7</v>
+      </c>
+      <c r="X9" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y9" t="s">
+        <v>9</v>
+      </c>
+      <c r="Z9" t="s">
+        <v>10</v>
+      </c>
+      <c r="AA9" t="s">
+        <v>11</v>
+      </c>
+      <c r="AB9" t="s">
+        <v>12</v>
+      </c>
+      <c r="AC9" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD9" t="s">
+        <v>14</v>
+      </c>
+      <c r="AE9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="P10">
+        <v>0</v>
+      </c>
+      <c r="Q10">
+        <v>11</v>
+      </c>
+      <c r="R10">
+        <v>1.9315485205580501E-2</v>
+      </c>
+      <c r="S10">
+        <v>0.18384910279441899</v>
+      </c>
+      <c r="T10">
+        <v>0</v>
+      </c>
+      <c r="U10">
+        <v>0</v>
+      </c>
+      <c r="V10">
+        <v>0</v>
+      </c>
+      <c r="W10">
+        <v>0</v>
+      </c>
+      <c r="X10">
+        <v>0</v>
+      </c>
+      <c r="Y10">
+        <v>612</v>
+      </c>
+      <c r="Z10" t="s">
         <v>32</v>
       </c>
-      <c r="L6" t="s">
+      <c r="AA10" t="s">
         <v>33</v>
       </c>
-      <c r="M6" t="s">
+      <c r="AB10" t="s">
         <v>34</v>
       </c>
-      <c r="N6">
-        <v>1358814.5036644801</v>
-      </c>
-      <c r="O6">
-        <v>635.54291778766299</v>
-      </c>
-      <c r="P6" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="AC10">
+        <v>1250133.6164057699</v>
+      </c>
+      <c r="AD10">
+        <v>551.86618428388397</v>
+      </c>
+      <c r="AE10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="B11">
         <v>2405000</v>
       </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P11">
+        <v>1</v>
+      </c>
+      <c r="Q11">
+        <v>11</v>
+      </c>
+      <c r="R11">
+        <v>1.3132735537354801E-2</v>
+      </c>
+      <c r="S11">
+        <v>0.16298649246264499</v>
+      </c>
+      <c r="T11">
+        <v>0</v>
+      </c>
+      <c r="U11">
+        <v>0</v>
+      </c>
+      <c r="V11">
+        <v>0</v>
+      </c>
+      <c r="W11">
+        <v>0</v>
+      </c>
+      <c r="X11">
+        <v>0</v>
+      </c>
+      <c r="Y11">
+        <v>612</v>
+      </c>
+      <c r="Z11" t="s">
+        <v>35</v>
+      </c>
+      <c r="AA11" t="s">
+        <v>36</v>
+      </c>
+      <c r="AB11" t="s">
+        <v>37</v>
+      </c>
+      <c r="AC11">
+        <v>1430073.88649123</v>
+      </c>
+      <c r="AD11">
+        <v>567.65540398927101</v>
+      </c>
+      <c r="AE11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="P12">
+        <v>0.236815999999999</v>
+      </c>
+      <c r="Q12">
+        <v>11</v>
+      </c>
+      <c r="R12">
+        <v>1.5760404146350701E-2</v>
+      </c>
+      <c r="S12">
+        <v>0.17185310185364899</v>
+      </c>
+      <c r="T12">
+        <v>0</v>
+      </c>
+      <c r="U12">
+        <v>0</v>
+      </c>
+      <c r="V12">
+        <v>0</v>
+      </c>
+      <c r="W12">
+        <v>0</v>
+      </c>
+      <c r="X12">
+        <v>0</v>
+      </c>
+      <c r="Y12">
+        <v>612</v>
+      </c>
+      <c r="Z12" t="s">
+        <v>38</v>
+      </c>
+      <c r="AA12" t="s">
+        <v>39</v>
+      </c>
+      <c r="AB12" t="s">
+        <v>40</v>
+      </c>
+      <c r="AC12">
+        <v>1114164.99970491</v>
+      </c>
+      <c r="AD12">
+        <v>560.94498561448097</v>
+      </c>
+      <c r="AE12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+      <c r="P13">
+        <v>0.41251199999999999</v>
+      </c>
+      <c r="Q13">
+        <v>11</v>
+      </c>
+      <c r="R13">
+        <v>1.46969712034159E-2</v>
+      </c>
+      <c r="S13">
+        <v>0.168264732876584</v>
+      </c>
+      <c r="T13">
+        <v>0</v>
+      </c>
+      <c r="U13">
+        <v>0</v>
+      </c>
+      <c r="V13">
+        <v>0</v>
+      </c>
+      <c r="W13">
+        <v>0</v>
+      </c>
+      <c r="X13">
+        <v>0</v>
+      </c>
+      <c r="Y13">
+        <v>612</v>
+      </c>
+      <c r="Z13" t="s">
+        <v>41</v>
+      </c>
+      <c r="AA13" t="s">
+        <v>42</v>
+      </c>
+      <c r="AB13" t="s">
+        <v>43</v>
+      </c>
+      <c r="AC13">
+        <v>1147731.49415961</v>
+      </c>
+      <c r="AD13">
+        <v>563.66073140380797</v>
+      </c>
+      <c r="AE13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>0</v>
       </c>
@@ -870,101 +1116,149 @@
       <c r="L14" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P14">
+        <v>0.18471199999999999</v>
+      </c>
+      <c r="Q14">
+        <v>11</v>
+      </c>
+      <c r="R14">
+        <v>1.63910446125097E-2</v>
+      </c>
+      <c r="S14">
+        <v>0.17398108810749</v>
+      </c>
+      <c r="T14">
+        <v>0</v>
+      </c>
+      <c r="U14">
+        <v>0</v>
+      </c>
+      <c r="V14">
+        <v>0</v>
+      </c>
+      <c r="W14">
+        <v>0</v>
+      </c>
+      <c r="X14">
+        <v>0</v>
+      </c>
+      <c r="Y14">
+        <v>612</v>
+      </c>
+      <c r="Z14" t="s">
+        <v>44</v>
+      </c>
+      <c r="AA14" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB14" t="s">
+        <v>46</v>
+      </c>
+      <c r="AC14">
+        <v>1131137.46015619</v>
+      </c>
+      <c r="AD14">
+        <v>559.33448520453203</v>
+      </c>
+      <c r="AE14" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A15">
         <f>$B$11*A2</f>
         <v>0</v>
       </c>
       <c r="B15">
-        <f t="shared" ref="B15:I15" si="0">$B$11*B2</f>
+        <f>$B$11*B2</f>
         <v>26455000</v>
       </c>
       <c r="C15">
-        <f t="shared" si="0"/>
-        <v>56435.143195352313</v>
+        <f>$B$11*C2</f>
+        <v>46453.741919421103</v>
       </c>
       <c r="D15">
-        <f t="shared" si="0"/>
-        <v>443362.34642464644</v>
+        <f>$B$11*D2</f>
+        <v>442157.09222057764</v>
       </c>
       <c r="E15">
-        <f t="shared" si="0"/>
+        <f>$B$11*E2</f>
         <v>0</v>
       </c>
       <c r="F15">
-        <f t="shared" si="0"/>
+        <f>$B$11*F2</f>
         <v>0</v>
       </c>
       <c r="G15">
-        <f t="shared" si="0"/>
+        <f>$B$11*G2</f>
         <v>0</v>
       </c>
       <c r="H15">
-        <f t="shared" si="0"/>
+        <f>$B$11*H2</f>
         <v>0</v>
       </c>
       <c r="I15">
-        <f t="shared" si="0"/>
+        <f>$B$11*I2</f>
         <v>0</v>
       </c>
       <c r="J15">
         <f>$B$11/1000*N2</f>
-        <v>3554134637.0932903</v>
+        <v>3006571347.4558768</v>
       </c>
       <c r="K15">
         <f>$B$11/1000*O2</f>
-        <v>1507763.8140363593</v>
+        <v>1327238.173202741</v>
       </c>
       <c r="L15" t="str">
         <f>P2</f>
         <v>none</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A16">
-        <f t="shared" ref="A16:I16" si="1">$B$11*A3</f>
+        <f>$B$11*A3</f>
         <v>2405000</v>
       </c>
       <c r="B16">
-        <f t="shared" si="1"/>
+        <f>$B$11*B3</f>
         <v>26455000</v>
       </c>
       <c r="C16">
-        <f t="shared" si="1"/>
-        <v>41565.630243269508</v>
+        <f>$B$11*C3</f>
+        <v>31584.228967338295</v>
       </c>
       <c r="D16">
-        <f t="shared" si="1"/>
-        <v>393187.76857672998</v>
+        <f>$B$11*D3</f>
+        <v>391982.51437266119</v>
       </c>
       <c r="E16">
-        <f t="shared" si="1"/>
+        <f>$B$11*E3</f>
         <v>0</v>
       </c>
       <c r="F16">
-        <f t="shared" si="1"/>
+        <f>$B$11*F3</f>
         <v>0</v>
       </c>
       <c r="G16">
-        <f t="shared" si="1"/>
+        <f>$B$11*G3</f>
         <v>0</v>
       </c>
       <c r="H16">
-        <f t="shared" si="1"/>
+        <f>$B$11*H3</f>
         <v>0</v>
       </c>
       <c r="I16">
-        <f t="shared" si="1"/>
+        <f>$B$11*I3</f>
         <v>0</v>
       </c>
       <c r="J16">
-        <f t="shared" ref="J16:J19" si="2">$B$11/1000*N3</f>
-        <v>3986890986.6488218</v>
+        <f>$B$11/1000*N3</f>
+        <v>3439327697.0114083</v>
       </c>
       <c r="K16">
-        <f t="shared" ref="K16:K19" si="3">$B$11/1000*O3</f>
-        <v>1551562.7638100809</v>
+        <f>$B$11/1000*O3</f>
+        <v>1365211.2465941969</v>
       </c>
       <c r="L16" t="str">
         <f>P3</f>
@@ -973,48 +1267,48 @@
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17">
-        <f t="shared" ref="A17:I17" si="4">$B$11*A4</f>
+        <f>$B$11*A4</f>
         <v>569542.47999999754</v>
       </c>
       <c r="B17">
-        <f t="shared" si="4"/>
+        <f>$B$11*B4</f>
         <v>26455000</v>
       </c>
       <c r="C17">
-        <f t="shared" si="4"/>
-        <v>47885.173247904648</v>
+        <f>$B$11*C4</f>
+        <v>37903.771971973438</v>
       </c>
       <c r="D17">
-        <f t="shared" si="4"/>
-        <v>414511.96416209463</v>
+        <f>$B$11*D4</f>
+        <v>413306.70995802584</v>
       </c>
       <c r="E17">
-        <f t="shared" si="4"/>
+        <f>$B$11*E4</f>
         <v>0</v>
       </c>
       <c r="F17">
-        <f t="shared" si="4"/>
+        <f>$B$11*F4</f>
         <v>0</v>
       </c>
       <c r="G17">
-        <f t="shared" si="4"/>
+        <f>$B$11*G4</f>
         <v>0</v>
       </c>
       <c r="H17">
-        <f t="shared" si="4"/>
+        <f>$B$11*H4</f>
         <v>0</v>
       </c>
       <c r="I17">
-        <f t="shared" si="4"/>
+        <f>$B$11*I4</f>
         <v>0</v>
       </c>
       <c r="J17">
-        <f t="shared" si="2"/>
-        <v>3227130113.927722</v>
+        <f>$B$11/1000*N4</f>
+        <v>2679566824.2903085</v>
       </c>
       <c r="K17">
-        <f t="shared" si="3"/>
-        <v>1532948.2101562477</v>
+        <f>$B$11/1000*O4</f>
+        <v>1349072.6904028268</v>
       </c>
       <c r="L17" t="str">
         <f>P4</f>
@@ -1023,48 +1317,48 @@
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18">
-        <f t="shared" ref="A18:I18" si="5">$B$11*A5</f>
+        <f>$B$11*A5</f>
         <v>992091.36</v>
       </c>
       <c r="B18">
-        <f t="shared" si="5"/>
+        <f>$B$11*B5</f>
         <v>26455000</v>
       </c>
       <c r="C18">
-        <f t="shared" si="5"/>
-        <v>45327.617020146456</v>
+        <f>$B$11*C5</f>
+        <v>35346.215744215238</v>
       </c>
       <c r="D18">
-        <f t="shared" si="5"/>
-        <v>405881.93677225331</v>
+        <f>$B$11*D5</f>
+        <v>404676.68256818451</v>
       </c>
       <c r="E18">
-        <f t="shared" si="5"/>
+        <f>$B$11*E5</f>
         <v>0</v>
       </c>
       <c r="F18">
-        <f t="shared" si="5"/>
+        <f>$B$11*F5</f>
         <v>0</v>
       </c>
       <c r="G18">
-        <f t="shared" si="5"/>
+        <f>$B$11*G5</f>
         <v>0</v>
       </c>
       <c r="H18">
-        <f t="shared" si="5"/>
+        <f>$B$11*H5</f>
         <v>0</v>
       </c>
       <c r="I18">
-        <f t="shared" si="5"/>
+        <f>$B$11*I5</f>
         <v>0</v>
       </c>
       <c r="J18">
-        <f t="shared" si="2"/>
-        <v>3307857533.0912757</v>
+        <f>$B$11/1000*N5</f>
+        <v>2760294243.4538622</v>
       </c>
       <c r="K18">
-        <f t="shared" si="3"/>
-        <v>1540481.6295173278</v>
+        <f>$B$11/1000*O5</f>
+        <v>1355604.0590261582</v>
       </c>
       <c r="L18" t="str">
         <f>P5</f>
@@ -1073,48 +1367,48 @@
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19">
-        <f t="shared" ref="A19:I19" si="6">$B$11*A6</f>
+        <f>$B$11*A6</f>
         <v>444232.36</v>
       </c>
       <c r="B19">
-        <f t="shared" si="6"/>
+        <f>$B$11*B6</f>
         <v>26455000</v>
       </c>
       <c r="C19">
-        <f t="shared" si="6"/>
-        <v>49401.863569017289</v>
+        <f>$B$11*C6</f>
+        <v>39420.462293085824</v>
       </c>
       <c r="D19">
-        <f t="shared" si="6"/>
-        <v>419629.77110258222</v>
+        <f>$B$11*D6</f>
+        <v>418424.51689851342</v>
       </c>
       <c r="E19">
-        <f t="shared" si="6"/>
+        <f>$B$11*E6</f>
         <v>0</v>
       </c>
       <c r="F19">
-        <f t="shared" si="6"/>
+        <f>$B$11*F6</f>
         <v>0</v>
       </c>
       <c r="G19">
-        <f t="shared" si="6"/>
+        <f>$B$11*G6</f>
         <v>0</v>
       </c>
       <c r="H19">
-        <f t="shared" si="6"/>
+        <f>$B$11*H6</f>
         <v>0</v>
       </c>
       <c r="I19">
-        <f t="shared" si="6"/>
+        <f>$B$11*I6</f>
         <v>0</v>
       </c>
       <c r="J19">
-        <f t="shared" si="2"/>
-        <v>3267948881.3130746</v>
+        <f>$B$11/1000*N6</f>
+        <v>2720385591.6756368</v>
       </c>
       <c r="K19">
-        <f t="shared" si="3"/>
-        <v>1528480.7172793294</v>
+        <f>$B$11/1000*O6</f>
+        <v>1345199.4369168996</v>
       </c>
       <c r="L19" t="str">
         <f>P6</f>
@@ -1127,31 +1421,31 @@
         <v>strategy</v>
       </c>
       <c r="C24" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="D24" t="s">
-        <v>42</v>
+        <v>27</v>
       </c>
       <c r="E24" t="s">
-        <v>39</v>
+        <v>24</v>
       </c>
       <c r="F24" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="H24" t="s">
         <v>15</v>
       </c>
       <c r="I24" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="J24" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="K24" t="s">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="L24" t="s">
-        <v>46</v>
+        <v>31</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
@@ -1161,38 +1455,38 @@
       </c>
       <c r="C25" s="2">
         <f>C15</f>
-        <v>56435.143195352313</v>
+        <v>46453.741919421103</v>
       </c>
       <c r="D25" s="2">
         <f>D15/1000</f>
-        <v>443.36234642464643</v>
+        <v>442.15709222057762</v>
       </c>
       <c r="E25" s="2">
         <f>J15/1000000</f>
-        <v>3554.1346370932902</v>
+        <v>3006.571347455877</v>
       </c>
       <c r="F25" s="2">
         <f>K15/1000</f>
-        <v>1507.7638140363592</v>
+        <v>1327.2381732027409</v>
       </c>
       <c r="H25" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="I25">
         <f>C2*1000</f>
-        <v>23.465756006383497</v>
+        <v>19.315485205580501</v>
       </c>
       <c r="J25">
         <f>D2*1000</f>
-        <v>184.35024799361599</v>
+        <v>183.849102794419</v>
       </c>
       <c r="K25">
         <f>N2</f>
-        <v>1477810.65991405</v>
+        <v>1250133.6164057699</v>
       </c>
       <c r="L25">
         <f>O2</f>
-        <v>626.92882080513903</v>
+        <v>551.86618428388397</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
@@ -1202,38 +1496,38 @@
       </c>
       <c r="C26" s="2">
         <f>C19</f>
-        <v>49401.863569017289</v>
+        <v>39420.462293085824</v>
       </c>
       <c r="D26" s="2">
         <f>D19/1000</f>
-        <v>419.6297711025822</v>
+        <v>418.42451689851345</v>
       </c>
       <c r="E26" s="2">
         <f>J19/1000000</f>
-        <v>3267.9488813130747</v>
+        <v>2720.385591675637</v>
       </c>
       <c r="F26" s="2">
         <f>K19/1000</f>
-        <v>1528.4807172793294</v>
+        <v>1345.1994369168997</v>
       </c>
       <c r="H26" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="I26">
-        <f t="shared" ref="I26:I29" si="7">C3*1000</f>
-        <v>17.283006338157801</v>
+        <f>C3*1000</f>
+        <v>13.132735537354801</v>
       </c>
       <c r="J26">
-        <f t="shared" ref="J26:J29" si="8">D3*1000</f>
-        <v>163.487637661842</v>
+        <f>D3*1000</f>
+        <v>162.98649246264497</v>
       </c>
       <c r="K26">
-        <f t="shared" ref="K26:L29" si="9">N3</f>
-        <v>1657750.9299995101</v>
+        <f>N3</f>
+        <v>1430073.88649123</v>
       </c>
       <c r="L26">
-        <f t="shared" si="9"/>
-        <v>645.14044233267396</v>
+        <f>O3</f>
+        <v>567.65540398927101</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
@@ -1243,38 +1537,38 @@
       </c>
       <c r="C27" s="2">
         <f>C17</f>
-        <v>47885.173247904648</v>
+        <v>37903.771971973438</v>
       </c>
       <c r="D27" s="2">
-        <f t="shared" ref="D27:D28" si="10">D17/1000</f>
-        <v>414.51196416209461</v>
+        <f t="shared" ref="D27:D28" si="0">D17/1000</f>
+        <v>413.30670995802586</v>
       </c>
       <c r="E27" s="2">
-        <f t="shared" ref="E27:E28" si="11">J17/1000000</f>
-        <v>3227.130113927722</v>
+        <f t="shared" ref="E27:E28" si="1">J17/1000000</f>
+        <v>2679.5668242903084</v>
       </c>
       <c r="F27" s="2">
-        <f t="shared" ref="F27:F28" si="12">K17/1000</f>
-        <v>1532.9482101562478</v>
+        <f t="shared" ref="F27:F28" si="2">K17/1000</f>
+        <v>1349.0726904028268</v>
       </c>
       <c r="H27" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="I27">
-        <f t="shared" si="7"/>
-        <v>19.910674947153698</v>
+        <f>C4*1000</f>
+        <v>15.760404146350702</v>
       </c>
       <c r="J27">
-        <f t="shared" si="8"/>
-        <v>172.35424705284601</v>
+        <f>D4*1000</f>
+        <v>171.85310185364898</v>
       </c>
       <c r="K27">
-        <f t="shared" si="9"/>
-        <v>1341842.04321319</v>
+        <f>N4</f>
+        <v>1114164.99970491</v>
       </c>
       <c r="L27">
-        <f t="shared" si="9"/>
-        <v>637.40050318347096</v>
+        <f>O4</f>
+        <v>560.94498561448097</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
@@ -1284,38 +1578,38 @@
       </c>
       <c r="C28" s="2">
         <f>C18</f>
-        <v>45327.617020146456</v>
+        <v>35346.215744215238</v>
       </c>
       <c r="D28" s="2">
-        <f t="shared" si="10"/>
-        <v>405.88193677225331</v>
+        <f t="shared" si="0"/>
+        <v>404.6766825681845</v>
       </c>
       <c r="E28" s="2">
-        <f t="shared" si="11"/>
-        <v>3307.8575330912759</v>
+        <f t="shared" si="1"/>
+        <v>2760.2942434538622</v>
       </c>
       <c r="F28" s="2">
-        <f t="shared" si="12"/>
-        <v>1540.4816295173277</v>
+        <f t="shared" si="2"/>
+        <v>1355.6040590261582</v>
       </c>
       <c r="H28" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="I28">
-        <f t="shared" si="7"/>
-        <v>18.847242004218899</v>
+        <f>C5*1000</f>
+        <v>14.696971203415901</v>
       </c>
       <c r="J28">
-        <f t="shared" si="8"/>
-        <v>168.76587807578099</v>
+        <f>D5*1000</f>
+        <v>168.26473287658399</v>
       </c>
       <c r="K28">
-        <f t="shared" si="9"/>
-        <v>1375408.5376678901</v>
+        <f>N5</f>
+        <v>1147731.49415961</v>
       </c>
       <c r="L28">
-        <f t="shared" si="9"/>
-        <v>640.53290208620695</v>
+        <f>O5</f>
+        <v>563.66073140380797</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
@@ -1325,47 +1619,47 @@
       </c>
       <c r="C29" s="2">
         <f>C16</f>
-        <v>41565.630243269508</v>
+        <v>31584.228967338295</v>
       </c>
       <c r="D29" s="2">
         <f>D16/1000</f>
-        <v>393.18776857672998</v>
+        <v>391.98251437266117</v>
       </c>
       <c r="E29" s="2">
         <f>J16/1000000</f>
-        <v>3986.890986648822</v>
+        <v>3439.3276970114084</v>
       </c>
       <c r="F29" s="2">
         <f>K16/1000</f>
-        <v>1551.5627638100809</v>
+        <v>1365.2112465941968</v>
       </c>
       <c r="H29" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="I29">
-        <f t="shared" si="7"/>
-        <v>20.541315413312802</v>
+        <f>C6*1000</f>
+        <v>16.391044612509699</v>
       </c>
       <c r="J29">
-        <f t="shared" si="8"/>
-        <v>174.48223330668699</v>
+        <f>D6*1000</f>
+        <v>173.98108810749</v>
       </c>
       <c r="K29">
-        <f t="shared" si="9"/>
-        <v>1358814.5036644801</v>
+        <f>N6</f>
+        <v>1131137.46015619</v>
       </c>
       <c r="L29">
-        <f t="shared" si="9"/>
-        <v>635.54291778766299</v>
+        <f>O6</f>
+        <v>559.33448520453203</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="D31" s="2">
         <f>C29-C28</f>
-        <v>-3761.9867768769473</v>
+        <v>-3761.9867768769436</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
@@ -1382,13 +1676,23 @@
         <v>679.03345355754618</v>
       </c>
     </row>
-    <row r="33" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C33">
         <f>F29-F28</f>
-        <v>11.081134292753177</v>
-      </c>
-    </row>
-    <row r="37" spans="3:4" x14ac:dyDescent="0.25">
+        <v>9.6071875680386256</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B35" s="2">
+        <f>C29-C25</f>
+        <v>-14869.512952082809</v>
+      </c>
+      <c r="D35" s="2">
+        <f>C28-C29</f>
+        <v>3761.9867768769436</v>
+      </c>
+    </row>
+    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D37" s="2"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
final version prior to submission for Annals. added in discounting (3% annually, done on a monthly cycle basis), converted stroke risk with therapy to an odds ratio (in comparison to prior, which was a percentage). Considerations for revisions: 1. risk of stroke up to a year for undiagnosed BCVI (currently x1 month/initial admission); 2. better utility values; 3. costs of nephrotoxicity/complications with CTA, although literature/evidence suggests that this is a non-factor (i.e. evidence suggests contrast-induced nephrotoxicity may be a myth)
</commit_message>
<xml_diff>
--- a/results/annual.data.united.states.xlsx
+++ b/results/annual.data.united.states.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ayman\Google Drive\research\trauma\CT.neck\code\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9380184E-4F16-4536-9AF1-2D0BAE6C4A15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B74C70E2-8CA3-40C2-B1EE-3AA7D281C98C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4065" yWindow="3120" windowWidth="20895" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="825" yWindow="-120" windowWidth="28095" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="50">
   <si>
     <t>ct.scan</t>
   </si>
@@ -105,21 +105,9 @@
     <t>Adjusted:</t>
   </si>
   <si>
-    <t>Universal vs. EDC</t>
-  </si>
-  <si>
     <t>Total cost, 1 year, in millions</t>
   </si>
   <si>
-    <t>Total QALY, 1 year, in thousands</t>
-  </si>
-  <si>
-    <t>Strokes, initial month event, IN THOUSANDS</t>
-  </si>
-  <si>
-    <t>Mortality, initial month event, in thousands</t>
-  </si>
-  <si>
     <t>Strokes per 1000</t>
   </si>
   <si>
@@ -175,6 +163,27 @@
   </si>
   <si>
     <t>[0.03407597456609395, 0.08668231303822965, 0.13927074907017586, 0.19184128879670004, 0.24439393835044254, 0.29692870386191755, 0.3494455914595137, 0.40194460726949494, 0.4544257574160011, 0.5068890480210488, 0.5593344852045322]</t>
+  </si>
+  <si>
+    <t>Strokes, initial month event</t>
+  </si>
+  <si>
+    <t>Mortality, initial month event</t>
+  </si>
+  <si>
+    <t>Total QALY, 1 year</t>
+  </si>
+  <si>
+    <t>Table One: Results of the Base Case Scenario</t>
+  </si>
+  <si>
+    <t>Strategy</t>
+  </si>
+  <si>
+    <t>Strokes Averted per Year</t>
+  </si>
+  <si>
+    <t>N/A</t>
   </si>
 </sst>
 </file>
@@ -498,10 +507,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AE37"/>
+  <dimension ref="A1:R40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G13" workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -510,17 +519,21 @@
     <col min="2" max="2" width="9.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="27.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="41.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="29.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.28515625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="41" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="40.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="29.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -570,7 +583,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -602,13 +615,13 @@
         <v>612</v>
       </c>
       <c r="K2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="L2" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="M2" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="N2">
         <v>1250133.6164057699</v>
@@ -620,7 +633,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -652,13 +665,13 @@
         <v>612</v>
       </c>
       <c r="K3" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="L3" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="M3" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="N3">
         <v>1430073.88649123</v>
@@ -670,7 +683,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>0.236815999999999</v>
       </c>
@@ -702,13 +715,13 @@
         <v>612</v>
       </c>
       <c r="K4" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="L4" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="M4" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="N4">
         <v>1114164.99970491</v>
@@ -720,7 +733,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>0.41251199999999999</v>
       </c>
@@ -752,13 +765,13 @@
         <v>612</v>
       </c>
       <c r="K5" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="L5" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="M5" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="N5">
         <v>1147731.49415961</v>
@@ -770,7 +783,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>0.18471199999999999</v>
       </c>
@@ -802,13 +815,13 @@
         <v>612</v>
       </c>
       <c r="K6" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="L6" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="M6" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="N6">
         <v>1131137.46015619</v>
@@ -820,266 +833,20 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="P9" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q9" t="s">
-        <v>1</v>
-      </c>
-      <c r="R9" t="s">
-        <v>2</v>
-      </c>
-      <c r="S9" t="s">
-        <v>3</v>
-      </c>
-      <c r="T9" t="s">
-        <v>4</v>
-      </c>
-      <c r="U9" t="s">
-        <v>5</v>
-      </c>
-      <c r="V9" t="s">
-        <v>6</v>
-      </c>
-      <c r="W9" t="s">
-        <v>7</v>
-      </c>
-      <c r="X9" t="s">
-        <v>8</v>
-      </c>
-      <c r="Y9" t="s">
-        <v>9</v>
-      </c>
-      <c r="Z9" t="s">
-        <v>10</v>
-      </c>
-      <c r="AA9" t="s">
-        <v>11</v>
-      </c>
-      <c r="AB9" t="s">
-        <v>12</v>
-      </c>
-      <c r="AC9" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD9" t="s">
-        <v>14</v>
-      </c>
-      <c r="AE9" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="P10">
-        <v>0</v>
-      </c>
-      <c r="Q10">
-        <v>11</v>
-      </c>
-      <c r="R10">
-        <v>1.9315485205580501E-2</v>
-      </c>
-      <c r="S10">
-        <v>0.18384910279441899</v>
-      </c>
-      <c r="T10">
-        <v>0</v>
-      </c>
-      <c r="U10">
-        <v>0</v>
-      </c>
-      <c r="V10">
-        <v>0</v>
-      </c>
-      <c r="W10">
-        <v>0</v>
-      </c>
-      <c r="X10">
-        <v>0</v>
-      </c>
-      <c r="Y10">
-        <v>612</v>
-      </c>
-      <c r="Z10" t="s">
-        <v>32</v>
-      </c>
-      <c r="AA10" t="s">
-        <v>33</v>
-      </c>
-      <c r="AB10" t="s">
-        <v>34</v>
-      </c>
-      <c r="AC10">
-        <v>1250133.6164057699</v>
-      </c>
-      <c r="AD10">
-        <v>551.86618428388397</v>
-      </c>
-      <c r="AE10" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>21</v>
       </c>
       <c r="B11">
         <v>2405000</v>
       </c>
-      <c r="P11">
-        <v>1</v>
-      </c>
-      <c r="Q11">
-        <v>11</v>
-      </c>
-      <c r="R11">
-        <v>1.3132735537354801E-2</v>
-      </c>
-      <c r="S11">
-        <v>0.16298649246264499</v>
-      </c>
-      <c r="T11">
-        <v>0</v>
-      </c>
-      <c r="U11">
-        <v>0</v>
-      </c>
-      <c r="V11">
-        <v>0</v>
-      </c>
-      <c r="W11">
-        <v>0</v>
-      </c>
-      <c r="X11">
-        <v>0</v>
-      </c>
-      <c r="Y11">
-        <v>612</v>
-      </c>
-      <c r="Z11" t="s">
-        <v>35</v>
-      </c>
-      <c r="AA11" t="s">
-        <v>36</v>
-      </c>
-      <c r="AB11" t="s">
-        <v>37</v>
-      </c>
-      <c r="AC11">
-        <v>1430073.88649123</v>
-      </c>
-      <c r="AD11">
-        <v>567.65540398927101</v>
-      </c>
-      <c r="AE11" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="12" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="P12">
-        <v>0.236815999999999</v>
-      </c>
-      <c r="Q12">
-        <v>11</v>
-      </c>
-      <c r="R12">
-        <v>1.5760404146350701E-2</v>
-      </c>
-      <c r="S12">
-        <v>0.17185310185364899</v>
-      </c>
-      <c r="T12">
-        <v>0</v>
-      </c>
-      <c r="U12">
-        <v>0</v>
-      </c>
-      <c r="V12">
-        <v>0</v>
-      </c>
-      <c r="W12">
-        <v>0</v>
-      </c>
-      <c r="X12">
-        <v>0</v>
-      </c>
-      <c r="Y12">
-        <v>612</v>
-      </c>
-      <c r="Z12" t="s">
-        <v>38</v>
-      </c>
-      <c r="AA12" t="s">
-        <v>39</v>
-      </c>
-      <c r="AB12" t="s">
-        <v>40</v>
-      </c>
-      <c r="AC12">
-        <v>1114164.99970491</v>
-      </c>
-      <c r="AD12">
-        <v>560.94498561448097</v>
-      </c>
-      <c r="AE12" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="13" spans="1:31" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>22</v>
       </c>
-      <c r="P13">
-        <v>0.41251199999999999</v>
-      </c>
-      <c r="Q13">
-        <v>11</v>
-      </c>
-      <c r="R13">
-        <v>1.46969712034159E-2</v>
-      </c>
-      <c r="S13">
-        <v>0.168264732876584</v>
-      </c>
-      <c r="T13">
-        <v>0</v>
-      </c>
-      <c r="U13">
-        <v>0</v>
-      </c>
-      <c r="V13">
-        <v>0</v>
-      </c>
-      <c r="W13">
-        <v>0</v>
-      </c>
-      <c r="X13">
-        <v>0</v>
-      </c>
-      <c r="Y13">
-        <v>612</v>
-      </c>
-      <c r="Z13" t="s">
-        <v>41</v>
-      </c>
-      <c r="AA13" t="s">
-        <v>42</v>
-      </c>
-      <c r="AB13" t="s">
-        <v>43</v>
-      </c>
-      <c r="AC13">
-        <v>1147731.49415961</v>
-      </c>
-      <c r="AD13">
-        <v>563.66073140380797</v>
-      </c>
-      <c r="AE13" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="14" spans="1:31" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>0</v>
       </c>
@@ -1116,98 +883,50 @@
       <c r="L14" t="s">
         <v>15</v>
       </c>
-      <c r="P14">
-        <v>0.18471199999999999</v>
-      </c>
-      <c r="Q14">
-        <v>11</v>
-      </c>
-      <c r="R14">
-        <v>1.63910446125097E-2</v>
-      </c>
-      <c r="S14">
-        <v>0.17398108810749</v>
-      </c>
-      <c r="T14">
-        <v>0</v>
-      </c>
-      <c r="U14">
-        <v>0</v>
-      </c>
-      <c r="V14">
-        <v>0</v>
-      </c>
-      <c r="W14">
-        <v>0</v>
-      </c>
-      <c r="X14">
-        <v>0</v>
-      </c>
-      <c r="Y14">
-        <v>612</v>
-      </c>
-      <c r="Z14" t="s">
-        <v>44</v>
-      </c>
-      <c r="AA14" t="s">
-        <v>45</v>
-      </c>
-      <c r="AB14" t="s">
-        <v>46</v>
-      </c>
-      <c r="AC14">
-        <v>1131137.46015619</v>
-      </c>
-      <c r="AD14">
-        <v>559.33448520453203</v>
-      </c>
-      <c r="AE14" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="15" spans="1:31" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15">
-        <f>$B$11*A2</f>
+        <f t="shared" ref="A15:I15" si="0">$B$11*A2</f>
         <v>0</v>
       </c>
       <c r="B15">
-        <f>$B$11*B2</f>
+        <f t="shared" si="0"/>
         <v>26455000</v>
       </c>
       <c r="C15">
-        <f>$B$11*C2</f>
+        <f t="shared" si="0"/>
         <v>46453.741919421103</v>
       </c>
       <c r="D15">
-        <f>$B$11*D2</f>
+        <f t="shared" si="0"/>
         <v>442157.09222057764</v>
       </c>
       <c r="E15">
-        <f>$B$11*E2</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F15">
-        <f>$B$11*F2</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G15">
-        <f>$B$11*G2</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H15">
-        <f>$B$11*H2</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I15">
-        <f>$B$11*I2</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J15">
-        <f>$B$11/1000*N2</f>
+        <f t="shared" ref="J15:K19" si="1">$B$11/1000*N2</f>
         <v>3006571347.4558768</v>
       </c>
       <c r="K15">
-        <f>$B$11/1000*O2</f>
+        <f t="shared" si="1"/>
         <v>1327238.173202741</v>
       </c>
       <c r="L15" t="str">
@@ -1215,49 +934,49 @@
         <v>none</v>
       </c>
     </row>
-    <row r="16" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16">
-        <f>$B$11*A3</f>
+        <f t="shared" ref="A16:I16" si="2">$B$11*A3</f>
         <v>2405000</v>
       </c>
       <c r="B16">
-        <f>$B$11*B3</f>
+        <f t="shared" si="2"/>
         <v>26455000</v>
       </c>
       <c r="C16">
-        <f>$B$11*C3</f>
+        <f t="shared" si="2"/>
         <v>31584.228967338295</v>
       </c>
       <c r="D16">
-        <f>$B$11*D3</f>
+        <f t="shared" si="2"/>
         <v>391982.51437266119</v>
       </c>
       <c r="E16">
-        <f>$B$11*E3</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F16">
-        <f>$B$11*F3</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G16">
-        <f>$B$11*G3</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="H16">
-        <f>$B$11*H3</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="I16">
-        <f>$B$11*I3</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J16">
-        <f>$B$11/1000*N3</f>
+        <f t="shared" si="1"/>
         <v>3439327697.0114083</v>
       </c>
       <c r="K16">
-        <f>$B$11/1000*O3</f>
+        <f t="shared" si="1"/>
         <v>1365211.2465941969</v>
       </c>
       <c r="L16" t="str">
@@ -1267,47 +986,47 @@
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17">
-        <f>$B$11*A4</f>
+        <f t="shared" ref="A17:I17" si="3">$B$11*A4</f>
         <v>569542.47999999754</v>
       </c>
       <c r="B17">
-        <f>$B$11*B4</f>
+        <f t="shared" si="3"/>
         <v>26455000</v>
       </c>
       <c r="C17">
-        <f>$B$11*C4</f>
+        <f t="shared" si="3"/>
         <v>37903.771971973438</v>
       </c>
       <c r="D17">
-        <f>$B$11*D4</f>
+        <f t="shared" si="3"/>
         <v>413306.70995802584</v>
       </c>
       <c r="E17">
-        <f>$B$11*E4</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="F17">
-        <f>$B$11*F4</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="G17">
-        <f>$B$11*G4</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H17">
-        <f>$B$11*H4</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I17">
-        <f>$B$11*I4</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="J17">
-        <f>$B$11/1000*N4</f>
+        <f t="shared" si="1"/>
         <v>2679566824.2903085</v>
       </c>
       <c r="K17">
-        <f>$B$11/1000*O4</f>
+        <f t="shared" si="1"/>
         <v>1349072.6904028268</v>
       </c>
       <c r="L17" t="str">
@@ -1317,47 +1036,47 @@
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18">
-        <f>$B$11*A5</f>
+        <f t="shared" ref="A18:I18" si="4">$B$11*A5</f>
         <v>992091.36</v>
       </c>
       <c r="B18">
-        <f>$B$11*B5</f>
+        <f t="shared" si="4"/>
         <v>26455000</v>
       </c>
       <c r="C18">
-        <f>$B$11*C5</f>
+        <f t="shared" si="4"/>
         <v>35346.215744215238</v>
       </c>
       <c r="D18">
-        <f>$B$11*D5</f>
+        <f t="shared" si="4"/>
         <v>404676.68256818451</v>
       </c>
       <c r="E18">
-        <f>$B$11*E5</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="F18">
-        <f>$B$11*F5</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="G18">
-        <f>$B$11*G5</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="H18">
-        <f>$B$11*H5</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="I18">
-        <f>$B$11*I5</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="J18">
-        <f>$B$11/1000*N5</f>
+        <f t="shared" si="1"/>
         <v>2760294243.4538622</v>
       </c>
       <c r="K18">
-        <f>$B$11/1000*O5</f>
+        <f t="shared" si="1"/>
         <v>1355604.0590261582</v>
       </c>
       <c r="L18" t="str">
@@ -1367,47 +1086,47 @@
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19">
-        <f>$B$11*A6</f>
+        <f t="shared" ref="A19:I19" si="5">$B$11*A6</f>
         <v>444232.36</v>
       </c>
       <c r="B19">
-        <f>$B$11*B6</f>
+        <f t="shared" si="5"/>
         <v>26455000</v>
       </c>
       <c r="C19">
-        <f>$B$11*C6</f>
+        <f t="shared" si="5"/>
         <v>39420.462293085824</v>
       </c>
       <c r="D19">
-        <f>$B$11*D6</f>
+        <f t="shared" si="5"/>
         <v>418424.51689851342</v>
       </c>
       <c r="E19">
-        <f>$B$11*E6</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="F19">
-        <f>$B$11*F6</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="G19">
-        <f>$B$11*G6</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="H19">
-        <f>$B$11*H6</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="I19">
-        <f>$B$11*I6</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="J19">
-        <f>$B$11/1000*N6</f>
+        <f t="shared" si="1"/>
         <v>2720385591.6756368</v>
       </c>
       <c r="K19">
-        <f>$B$11/1000*O6</f>
+        <f t="shared" si="1"/>
         <v>1345199.4369168996</v>
       </c>
       <c r="L19" t="str">
@@ -1421,31 +1140,31 @@
         <v>strategy</v>
       </c>
       <c r="C24" t="s">
-        <v>26</v>
+        <v>43</v>
       </c>
       <c r="D24" t="s">
-        <v>27</v>
+        <v>44</v>
       </c>
       <c r="E24" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F24" t="s">
-        <v>25</v>
+        <v>45</v>
       </c>
       <c r="H24" t="s">
         <v>15</v>
       </c>
       <c r="I24" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="J24" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="K24" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="L24" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
@@ -1458,242 +1177,300 @@
         <v>46453.741919421103</v>
       </c>
       <c r="D25" s="2">
-        <f>D15/1000</f>
-        <v>442.15709222057762</v>
+        <f>D15</f>
+        <v>442157.09222057764</v>
       </c>
       <c r="E25" s="2">
         <f>J15/1000000</f>
         <v>3006.571347455877</v>
       </c>
       <c r="F25" s="2">
-        <f>K15/1000</f>
-        <v>1327.2381732027409</v>
-      </c>
-      <c r="H25" t="s">
-        <v>16</v>
+        <f>K15</f>
+        <v>1327238.173202741</v>
+      </c>
+      <c r="H25" t="str">
+        <f>B25</f>
+        <v>none</v>
       </c>
       <c r="I25">
-        <f>C2*1000</f>
+        <f t="shared" ref="I25:J29" si="6">C2*1000</f>
         <v>19.315485205580501</v>
       </c>
       <c r="J25">
-        <f>D2*1000</f>
+        <f t="shared" si="6"/>
         <v>183.849102794419</v>
       </c>
       <c r="K25">
-        <f>N2</f>
+        <f t="shared" ref="K25:L29" si="7">N2</f>
         <v>1250133.6164057699</v>
       </c>
       <c r="L25">
-        <f>O2</f>
+        <f t="shared" si="7"/>
         <v>551.86618428388397</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B26" t="str">
-        <f>L19</f>
-        <v>mc</v>
+        <f t="shared" ref="B26:B29" si="8">L16</f>
+        <v>universal</v>
       </c>
       <c r="C26" s="2">
-        <f>C19</f>
-        <v>39420.462293085824</v>
+        <f t="shared" ref="C26:D29" si="9">C16</f>
+        <v>31584.228967338295</v>
       </c>
       <c r="D26" s="2">
-        <f>D19/1000</f>
-        <v>418.42451689851345</v>
+        <f t="shared" si="9"/>
+        <v>391982.51437266119</v>
       </c>
       <c r="E26" s="2">
-        <f>J19/1000000</f>
-        <v>2720.385591675637</v>
+        <f t="shared" ref="E26:E29" si="10">J16/1000000</f>
+        <v>3439.3276970114084</v>
       </c>
       <c r="F26" s="2">
-        <f>K19/1000</f>
-        <v>1345.1994369168997</v>
-      </c>
-      <c r="H26" t="s">
-        <v>17</v>
+        <f t="shared" ref="F26:F29" si="11">K16</f>
+        <v>1365211.2465941969</v>
+      </c>
+      <c r="H26" t="str">
+        <f t="shared" ref="H26:H29" si="12">B26</f>
+        <v>universal</v>
       </c>
       <c r="I26">
-        <f>C3*1000</f>
+        <f t="shared" ref="I26:I29" si="13">C3*1000</f>
         <v>13.132735537354801</v>
       </c>
       <c r="J26">
-        <f>D3*1000</f>
+        <f t="shared" ref="J26:J29" si="14">D3*1000</f>
         <v>162.98649246264497</v>
       </c>
       <c r="K26">
-        <f>N3</f>
+        <f t="shared" si="7"/>
         <v>1430073.88649123</v>
       </c>
       <c r="L26">
-        <f>O3</f>
+        <f t="shared" si="7"/>
         <v>567.65540398927101</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B27" t="str">
-        <f>L17</f>
+        <f t="shared" si="8"/>
         <v>dc</v>
       </c>
       <c r="C27" s="2">
-        <f>C17</f>
+        <f t="shared" si="9"/>
         <v>37903.771971973438</v>
       </c>
       <c r="D27" s="2">
-        <f t="shared" ref="D27:D28" si="0">D17/1000</f>
-        <v>413.30670995802586</v>
+        <f t="shared" si="9"/>
+        <v>413306.70995802584</v>
       </c>
       <c r="E27" s="2">
-        <f t="shared" ref="E27:E28" si="1">J17/1000000</f>
+        <f t="shared" si="10"/>
         <v>2679.5668242903084</v>
       </c>
       <c r="F27" s="2">
-        <f t="shared" ref="F27:F28" si="2">K17/1000</f>
-        <v>1349.0726904028268</v>
-      </c>
-      <c r="H27" t="s">
-        <v>18</v>
+        <f t="shared" si="11"/>
+        <v>1349072.6904028268</v>
+      </c>
+      <c r="H27" t="str">
+        <f t="shared" si="12"/>
+        <v>dc</v>
       </c>
       <c r="I27">
-        <f>C4*1000</f>
+        <f t="shared" si="13"/>
         <v>15.760404146350702</v>
       </c>
       <c r="J27">
-        <f>D4*1000</f>
+        <f t="shared" si="14"/>
         <v>171.85310185364898</v>
       </c>
       <c r="K27">
-        <f>N4</f>
+        <f t="shared" si="7"/>
         <v>1114164.99970491</v>
       </c>
       <c r="L27">
-        <f>O4</f>
+        <f t="shared" si="7"/>
         <v>560.94498561448097</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B28" t="str">
-        <f>L18</f>
+        <f t="shared" si="8"/>
         <v>edc</v>
       </c>
       <c r="C28" s="2">
-        <f>C18</f>
+        <f t="shared" si="9"/>
         <v>35346.215744215238</v>
       </c>
       <c r="D28" s="2">
-        <f t="shared" si="0"/>
-        <v>404.6766825681845</v>
+        <f t="shared" si="9"/>
+        <v>404676.68256818451</v>
       </c>
       <c r="E28" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="10"/>
         <v>2760.2942434538622</v>
       </c>
       <c r="F28" s="2">
-        <f t="shared" si="2"/>
-        <v>1355.6040590261582</v>
-      </c>
-      <c r="H28" t="s">
-        <v>19</v>
+        <f t="shared" si="11"/>
+        <v>1355604.0590261582</v>
+      </c>
+      <c r="H28" t="str">
+        <f t="shared" si="12"/>
+        <v>edc</v>
       </c>
       <c r="I28">
-        <f>C5*1000</f>
+        <f t="shared" si="13"/>
         <v>14.696971203415901</v>
       </c>
       <c r="J28">
-        <f>D5*1000</f>
+        <f t="shared" si="14"/>
         <v>168.26473287658399</v>
       </c>
       <c r="K28">
-        <f>N5</f>
+        <f t="shared" si="7"/>
         <v>1147731.49415961</v>
       </c>
       <c r="L28">
-        <f>O5</f>
+        <f t="shared" si="7"/>
         <v>563.66073140380797</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B29" t="str">
-        <f>L16</f>
+        <f t="shared" si="8"/>
+        <v>mc</v>
+      </c>
+      <c r="C29" s="2">
+        <f t="shared" si="9"/>
+        <v>39420.462293085824</v>
+      </c>
+      <c r="D29" s="2">
+        <f t="shared" si="9"/>
+        <v>418424.51689851342</v>
+      </c>
+      <c r="E29" s="2">
+        <f t="shared" si="10"/>
+        <v>2720.385591675637</v>
+      </c>
+      <c r="F29" s="2">
+        <f t="shared" si="11"/>
+        <v>1345199.4369168996</v>
+      </c>
+      <c r="H29" t="str">
+        <f t="shared" si="12"/>
+        <v>mc</v>
+      </c>
+      <c r="I29">
+        <f t="shared" si="13"/>
+        <v>16.391044612509699</v>
+      </c>
+      <c r="J29">
+        <f t="shared" si="14"/>
+        <v>173.98108810749</v>
+      </c>
+      <c r="K29">
+        <f t="shared" si="7"/>
+        <v>1131137.46015619</v>
+      </c>
+      <c r="L29">
+        <f t="shared" si="7"/>
+        <v>559.33448520453203</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D31" s="2"/>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C32" s="1"/>
+      <c r="D32" s="3"/>
+      <c r="E32" t="s">
+        <v>46</v>
+      </c>
+      <c r="F32" s="2"/>
+    </row>
+    <row r="34" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="E34" t="s">
+        <v>47</v>
+      </c>
+      <c r="F34" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="35" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B35" s="2"/>
+      <c r="D35" s="2"/>
+      <c r="E35" t="str">
+        <f>B25</f>
+        <v>none</v>
+      </c>
+      <c r="F35" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="36" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="E36" t="str">
+        <f t="shared" ref="E36:E39" si="15">B26</f>
         <v>universal</v>
       </c>
-      <c r="C29" s="2">
-        <f>C16</f>
-        <v>31584.228967338295</v>
-      </c>
-      <c r="D29" s="2">
-        <f>D16/1000</f>
-        <v>391.98251437266117</v>
-      </c>
-      <c r="E29" s="2">
-        <f>J16/1000000</f>
-        <v>3439.3276970114084</v>
-      </c>
-      <c r="F29" s="2">
-        <f>K16/1000</f>
-        <v>1365.2112465941968</v>
-      </c>
-      <c r="H29" t="s">
-        <v>20</v>
-      </c>
-      <c r="I29">
-        <f>C6*1000</f>
-        <v>16.391044612509699</v>
-      </c>
-      <c r="J29">
-        <f>D6*1000</f>
-        <v>173.98108810749</v>
-      </c>
-      <c r="K29">
-        <f>N6</f>
-        <v>1131137.46015619</v>
-      </c>
-      <c r="L29">
-        <f>O6</f>
-        <v>559.33448520453203</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B31" t="s">
-        <v>23</v>
-      </c>
-      <c r="D31" s="2">
-        <f>C29-C28</f>
-        <v>-3761.9867768769436</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C32" s="1">
-        <f>E29-E28</f>
-        <v>679.03345355754618</v>
-      </c>
-      <c r="D32" s="3">
-        <f>(D29-D28)*1000</f>
-        <v>-12694.168195523333</v>
-      </c>
-      <c r="F32" s="2">
-        <f>E29-E28</f>
-        <v>679.03345355754618</v>
-      </c>
-    </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C33">
-        <f>F29-F28</f>
-        <v>9.6071875680386256</v>
-      </c>
-    </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B35" s="2">
-        <f>C29-C25</f>
-        <v>-14869.512952082809</v>
-      </c>
-      <c r="D35" s="2">
-        <f>C28-C29</f>
-        <v>3761.9867768769436</v>
-      </c>
-    </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="F36" s="2">
+        <f>$C$25-C26</f>
+        <v>14869.512952082809</v>
+      </c>
+      <c r="N36" s="2"/>
+      <c r="O36" s="2"/>
+      <c r="P36" s="2"/>
+      <c r="Q36" s="2"/>
+      <c r="R36" s="2"/>
+    </row>
+    <row r="37" spans="2:18" x14ac:dyDescent="0.25">
       <c r="D37" s="2"/>
+      <c r="E37" t="str">
+        <f t="shared" si="15"/>
+        <v>dc</v>
+      </c>
+      <c r="F37" s="2">
+        <f t="shared" ref="F37:F39" si="16">$C$25-C27</f>
+        <v>8549.9699474476656</v>
+      </c>
+      <c r="N37" s="2"/>
+      <c r="O37" s="2"/>
+      <c r="P37" s="2"/>
+      <c r="Q37" s="2"/>
+      <c r="R37" s="2"/>
+    </row>
+    <row r="38" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="E38" t="str">
+        <f t="shared" si="15"/>
+        <v>edc</v>
+      </c>
+      <c r="F38" s="2">
+        <f t="shared" si="16"/>
+        <v>11107.526175205865</v>
+      </c>
+      <c r="N38" s="2"/>
+      <c r="O38" s="2"/>
+      <c r="P38" s="2"/>
+      <c r="Q38" s="2"/>
+    </row>
+    <row r="39" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="E39" t="str">
+        <f t="shared" si="15"/>
+        <v>mc</v>
+      </c>
+      <c r="F39" s="2">
+        <f t="shared" si="16"/>
+        <v>7033.2796263352793</v>
+      </c>
+      <c r="N39" s="2"/>
+      <c r="O39" s="2"/>
+      <c r="P39" s="2"/>
+      <c r="Q39" s="2"/>
+    </row>
+    <row r="40" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="N40" s="2"/>
+      <c r="O40" s="2"/>
+      <c r="P40" s="2"/>
+      <c r="Q40" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>